<commit_message>
Fix calcolo peso ordini TAB e allineamento decimali (Order Tab)
</commit_message>
<xml_diff>
--- a/templates/Excel_per_INVIO_ORDINE.xlsx
+++ b/templates/Excel_per_INVIO_ORDINE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comme\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tammaro\riordino-bar\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBC8077-2259-402E-A878-6A580973CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,8 +45,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,6 +60,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -102,16 +112,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,26 +440,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>